<commit_message>
attdence 7 Jan 2024
</commit_message>
<xml_diff>
--- a/Angular B10 B2.xlsx
+++ b/Angular B10 B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Angular\javascript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A105C60F-1C8D-42AC-835C-8FC57C2BBA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD17764C-6698-4BEC-A59C-B7A0F55E718D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -29,11 +29,22 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={8D88C115-F3D9-48BB-8785-CB7D0D2CF01A}</author>
     <author>tc={8783CE86-BDB9-42C8-AC71-2AAF5C3DC86E}</author>
     <author>tc={37976732-7168-4646-8092-627EDB32F958}</author>
+    <author>tc={AAF149A4-F3B5-465F-B672-9517F63F11BE}</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{8783CE86-BDB9-42C8-AC71-2AAF5C3DC86E}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{8D88C115-F3D9-48BB-8785-CB7D0D2CF01A}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not feeling well reason cold and fever
+</t>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="1" shapeId="0" xr:uid="{8783CE86-BDB9-42C8-AC71-2AAF5C3DC86E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -41,7 +52,7 @@
     Medical Emergency</t>
       </text>
     </comment>
-    <comment ref="G5" authorId="1" shapeId="0" xr:uid="{37976732-7168-4646-8092-627EDB32F958}">
+    <comment ref="G5" authorId="2" shapeId="0" xr:uid="{37976732-7168-4646-8092-627EDB32F958}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -50,12 +61,20 @@
 </t>
       </text>
     </comment>
+    <comment ref="I5" authorId="3" shapeId="0" xr:uid="{AAF149A4-F3B5-465F-B672-9517F63F11BE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Medical emergency</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="13">
   <si>
     <t>Student Name</t>
   </si>
@@ -498,12 +517,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I3" dT="2024-01-07T16:22:45.44" personId="{D346A3DA-9822-4582-ACAA-5AEDCCB210ED}" id="{8D88C115-F3D9-48BB-8785-CB7D0D2CF01A}">
+    <text xml:space="preserve">Not feeling well reason cold and fever
+</text>
+  </threadedComment>
   <threadedComment ref="F5" dT="2024-01-04T16:30:19.91" personId="{D346A3DA-9822-4582-ACAA-5AEDCCB210ED}" id="{8783CE86-BDB9-42C8-AC71-2AAF5C3DC86E}">
     <text>Medical Emergency</text>
   </threadedComment>
   <threadedComment ref="G5" dT="2024-01-05T17:22:55.77" personId="{D346A3DA-9822-4582-ACAA-5AEDCCB210ED}" id="{37976732-7168-4646-8092-627EDB32F958}">
     <text xml:space="preserve">Medical emergency
 </text>
+  </threadedComment>
+  <threadedComment ref="I5" dT="2024-01-07T16:23:22.73" personId="{D346A3DA-9822-4582-ACAA-5AEDCCB210ED}" id="{AAF149A4-F3B5-465F-B672-9517F63F11BE}">
+    <text>Medical emergency</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -763,10 +789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D1CC70-9438-1A44-9A3A-851EC2F4124C}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -774,7 +800,7 @@
     <col min="2" max="2" width="19.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -797,10 +823,15 @@
         <v>45296</v>
       </c>
       <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="I1" s="4">
+        <v>45298</v>
+      </c>
       <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -823,10 +854,15 @@
         <v>2</v>
       </c>
       <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -849,10 +885,15 @@
         <v>2</v>
       </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -875,10 +916,15 @@
         <v>2</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -901,10 +947,15 @@
         <v>12</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -927,10 +978,15 @@
         <v>3</v>
       </c>
       <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -953,10 +1009,15 @@
         <v>2</v>
       </c>
       <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -977,12 +1038,17 @@
         <v>3</v>
       </c>
       <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:J8" xr:uid="{3DB7E5D7-F13D-8049-AED0-F89F0EA89AAF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:M8" xr:uid="{3DB7E5D7-F13D-8049-AED0-F89F0EA89AAF}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
attdence 23-Jan-24 and 24-Jan-24
</commit_message>
<xml_diff>
--- a/Angular B10 B2.xlsx
+++ b/Angular B10 B2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Angular\javascript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC08B16-4EDA-4EB5-BC52-E73B8721EB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731ACB4A-1A74-490B-9B7B-DDC4605FD184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F43F5E3C-0558-E346-B770-8540CD6B4863}"/>
   </bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="13">
   <si>
     <t>Student Name</t>
   </si>
@@ -797,10 +797,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D1CC70-9438-1A44-9A3A-851EC2F4124C}">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -808,7 +808,7 @@
     <col min="2" max="2" width="19.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -869,12 +869,20 @@
         <v>45312</v>
       </c>
       <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
+      <c r="Y1" s="4">
+        <v>45314</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>45315</v>
+      </c>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
-    </row>
-    <row r="2" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+    </row>
+    <row r="2" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -935,12 +943,20 @@
         <v>2</v>
       </c>
       <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
+      <c r="Y2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA2" s="7"/>
       <c r="AB2" s="7"/>
-    </row>
-    <row r="3" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+    </row>
+    <row r="3" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1001,12 +1017,20 @@
         <v>2</v>
       </c>
       <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
+      <c r="Y3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
-    </row>
-    <row r="4" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+    </row>
+    <row r="4" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1067,12 +1091,20 @@
         <v>3</v>
       </c>
       <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
+      <c r="Y4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
-    </row>
-    <row r="5" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1133,12 +1165,20 @@
         <v>3</v>
       </c>
       <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
+      <c r="Y5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
-    </row>
-    <row r="6" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1199,12 +1239,20 @@
         <v>3</v>
       </c>
       <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
+      <c r="Y6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
-    </row>
-    <row r="7" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1265,12 +1313,20 @@
         <v>2</v>
       </c>
       <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
+      <c r="Y7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="AA7" s="7"/>
       <c r="AB7" s="7"/>
-    </row>
-    <row r="8" spans="1:28" ht="18" x14ac:dyDescent="0.35">
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:32" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1329,14 +1385,22 @@
         <v>3</v>
       </c>
       <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
+      <c r="Y8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:AB8" xr:uid="{3DB7E5D7-F13D-8049-AED0-F89F0EA89AAF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:AF8" xr:uid="{3DB7E5D7-F13D-8049-AED0-F89F0EA89AAF}">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>